<commit_message>
substract 19 to the stock series
</commit_message>
<xml_diff>
--- a/week_02/data_input/MFA_II_tutorial_II.xlsx
+++ b/week_02/data_input/MFA_II_tutorial_II.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="inflow_driven" sheetId="1" state="visible" r:id="rId3"/>
@@ -504,11 +504,11 @@
           </c:spPr>
         </c:hiLowLines>
         <c:marker val="0"/>
-        <c:axId val="90280585"/>
-        <c:axId val="39919291"/>
+        <c:axId val="62275712"/>
+        <c:axId val="44196623"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="90280585"/>
+        <c:axId val="62275712"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -540,7 +540,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="39919291"/>
+        <c:crossAx val="44196623"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -548,7 +548,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="39919291"/>
+        <c:axId val="44196623"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -587,7 +587,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="90280585"/>
+        <c:crossAx val="62275712"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -626,9 +626,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>12</xdr:col>
-      <xdr:colOff>421560</xdr:colOff>
+      <xdr:colOff>421200</xdr:colOff>
       <xdr:row>19</xdr:row>
-      <xdr:rowOff>4320</xdr:rowOff>
+      <xdr:rowOff>3960</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -637,7 +637,7 @@
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="3769920" y="729720"/>
-        <a:ext cx="4904280" cy="2712960"/>
+        <a:ext cx="4903920" cy="2712600"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -829,7 +829,7 @@
   </sheetPr>
   <dimension ref="A1:D62"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="C10" activeCellId="0" sqref="C10"/>
     </sheetView>
   </sheetViews>
@@ -1416,8 +1416,8 @@
   </sheetPr>
   <dimension ref="A1:D62"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A25" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F54" activeCellId="0" sqref="F54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.59765625" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1441,7 +1441,7 @@
         <v>1990</v>
       </c>
       <c r="B2" s="1" t="n">
-        <v>20</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1450,7 +1450,7 @@
         <v>1991</v>
       </c>
       <c r="B3" s="1" t="n">
-        <v>21</v>
+        <v>2</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1459,7 +1459,7 @@
         <v>1992</v>
       </c>
       <c r="B4" s="1" t="n">
-        <v>30</v>
+        <v>11</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1468,7 +1468,7 @@
         <v>1993</v>
       </c>
       <c r="B5" s="1" t="n">
-        <v>39</v>
+        <v>20</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1477,7 +1477,7 @@
         <v>1994</v>
       </c>
       <c r="B6" s="1" t="n">
-        <v>45</v>
+        <v>26</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1486,7 +1486,7 @@
         <v>1995</v>
       </c>
       <c r="B7" s="1" t="n">
-        <v>50</v>
+        <v>31</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1495,7 +1495,7 @@
         <v>1996</v>
       </c>
       <c r="B8" s="1" t="n">
-        <v>51</v>
+        <v>32</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1504,7 +1504,7 @@
         <v>1997</v>
       </c>
       <c r="B9" s="1" t="n">
-        <v>52</v>
+        <v>33</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1513,7 +1513,7 @@
         <v>1998</v>
       </c>
       <c r="B10" s="1" t="n">
-        <v>100</v>
+        <v>81</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1522,8 +1522,7 @@
         <v>1999</v>
       </c>
       <c r="B11" s="1" t="n">
-        <f aca="false">B10+13</f>
-        <v>113</v>
+        <v>94</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1532,8 +1531,7 @@
         <v>2000</v>
       </c>
       <c r="B12" s="1" t="n">
-        <f aca="false">B11+13</f>
-        <v>126</v>
+        <v>107</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1542,8 +1540,7 @@
         <v>2001</v>
       </c>
       <c r="B13" s="1" t="n">
-        <f aca="false">B12+13</f>
-        <v>139</v>
+        <v>120</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1552,8 +1549,7 @@
         <v>2002</v>
       </c>
       <c r="B14" s="1" t="n">
-        <f aca="false">B13+13</f>
-        <v>152</v>
+        <v>133</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1562,8 +1558,7 @@
         <v>2003</v>
       </c>
       <c r="B15" s="1" t="n">
-        <f aca="false">B14+13</f>
-        <v>165</v>
+        <v>146</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1572,8 +1567,7 @@
         <v>2004</v>
       </c>
       <c r="B16" s="1" t="n">
-        <f aca="false">B15+13</f>
-        <v>178</v>
+        <v>159</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1582,8 +1576,7 @@
         <v>2005</v>
       </c>
       <c r="B17" s="1" t="n">
-        <f aca="false">B16+13</f>
-        <v>191</v>
+        <v>172</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1592,8 +1585,7 @@
         <v>2006</v>
       </c>
       <c r="B18" s="1" t="n">
-        <f aca="false">B17+13</f>
-        <v>204</v>
+        <v>185</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1602,8 +1594,7 @@
         <v>2007</v>
       </c>
       <c r="B19" s="1" t="n">
-        <f aca="false">B18+13</f>
-        <v>217</v>
+        <v>198</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1612,8 +1603,7 @@
         <v>2008</v>
       </c>
       <c r="B20" s="1" t="n">
-        <f aca="false">B19+13</f>
-        <v>230</v>
+        <v>211</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1622,8 +1612,7 @@
         <v>2009</v>
       </c>
       <c r="B21" s="1" t="n">
-        <f aca="false">B20+13</f>
-        <v>243</v>
+        <v>224</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1632,8 +1621,7 @@
         <v>2010</v>
       </c>
       <c r="B22" s="1" t="n">
-        <f aca="false">B21+13</f>
-        <v>256</v>
+        <v>237</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1642,8 +1630,7 @@
         <v>2011</v>
       </c>
       <c r="B23" s="1" t="n">
-        <f aca="false">B22+13</f>
-        <v>269</v>
+        <v>250</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1652,8 +1639,7 @@
         <v>2012</v>
       </c>
       <c r="B24" s="1" t="n">
-        <f aca="false">B23+13</f>
-        <v>282</v>
+        <v>263</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1662,8 +1648,7 @@
         <v>2013</v>
       </c>
       <c r="B25" s="1" t="n">
-        <f aca="false">B24+13</f>
-        <v>295</v>
+        <v>276</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1672,8 +1657,7 @@
         <v>2014</v>
       </c>
       <c r="B26" s="1" t="n">
-        <f aca="false">B25+13</f>
-        <v>308</v>
+        <v>289</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1682,8 +1666,7 @@
         <v>2015</v>
       </c>
       <c r="B27" s="1" t="n">
-        <f aca="false">B26+13</f>
-        <v>321</v>
+        <v>302</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1692,8 +1675,7 @@
         <v>2016</v>
       </c>
       <c r="B28" s="1" t="n">
-        <f aca="false">B27+13</f>
-        <v>334</v>
+        <v>315</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1702,8 +1684,7 @@
         <v>2017</v>
       </c>
       <c r="B29" s="1" t="n">
-        <f aca="false">B28+13</f>
-        <v>347</v>
+        <v>328</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1712,8 +1693,7 @@
         <v>2018</v>
       </c>
       <c r="B30" s="1" t="n">
-        <f aca="false">B29+13</f>
-        <v>360</v>
+        <v>341</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1722,8 +1702,7 @@
         <v>2019</v>
       </c>
       <c r="B31" s="1" t="n">
-        <f aca="false">B30+13</f>
-        <v>373</v>
+        <v>354</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1732,8 +1711,7 @@
         <v>2020</v>
       </c>
       <c r="B32" s="1" t="n">
-        <f aca="false">B31+13</f>
-        <v>386</v>
+        <v>367</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1742,8 +1720,7 @@
         <v>2021</v>
       </c>
       <c r="B33" s="1" t="n">
-        <f aca="false">B32+13</f>
-        <v>399</v>
+        <v>380</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1752,8 +1729,7 @@
         <v>2022</v>
       </c>
       <c r="B34" s="1" t="n">
-        <f aca="false">B33+13</f>
-        <v>412</v>
+        <v>393</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1762,8 +1738,7 @@
         <v>2023</v>
       </c>
       <c r="B35" s="1" t="n">
-        <f aca="false">B34+13</f>
-        <v>425</v>
+        <v>406</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1772,8 +1747,7 @@
         <v>2024</v>
       </c>
       <c r="B36" s="1" t="n">
-        <f aca="false">B35+13</f>
-        <v>438</v>
+        <v>419</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1782,8 +1756,7 @@
         <v>2025</v>
       </c>
       <c r="B37" s="1" t="n">
-        <f aca="false">B36+13</f>
-        <v>451</v>
+        <v>432</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1792,8 +1765,7 @@
         <v>2026</v>
       </c>
       <c r="B38" s="1" t="n">
-        <f aca="false">B37+13</f>
-        <v>464</v>
+        <v>445</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1802,8 +1774,7 @@
         <v>2027</v>
       </c>
       <c r="B39" s="1" t="n">
-        <f aca="false">B38+13</f>
-        <v>477</v>
+        <v>458</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1812,8 +1783,7 @@
         <v>2028</v>
       </c>
       <c r="B40" s="1" t="n">
-        <f aca="false">B39+13</f>
-        <v>490</v>
+        <v>471</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1822,8 +1792,7 @@
         <v>2029</v>
       </c>
       <c r="B41" s="1" t="n">
-        <f aca="false">B40+13</f>
-        <v>503</v>
+        <v>484</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1832,8 +1801,7 @@
         <v>2030</v>
       </c>
       <c r="B42" s="1" t="n">
-        <f aca="false">B41+13</f>
-        <v>516</v>
+        <v>497</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1842,8 +1810,7 @@
         <v>2031</v>
       </c>
       <c r="B43" s="1" t="n">
-        <f aca="false">B42+13</f>
-        <v>529</v>
+        <v>510</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1852,8 +1819,7 @@
         <v>2032</v>
       </c>
       <c r="B44" s="1" t="n">
-        <f aca="false">B43+13</f>
-        <v>542</v>
+        <v>523</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1862,8 +1828,7 @@
         <v>2033</v>
       </c>
       <c r="B45" s="1" t="n">
-        <f aca="false">B44+13</f>
-        <v>555</v>
+        <v>536</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1872,8 +1837,7 @@
         <v>2034</v>
       </c>
       <c r="B46" s="1" t="n">
-        <f aca="false">B45+13</f>
-        <v>568</v>
+        <v>549</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1882,8 +1846,7 @@
         <v>2035</v>
       </c>
       <c r="B47" s="1" t="n">
-        <f aca="false">B46+13</f>
-        <v>581</v>
+        <v>562</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1892,8 +1855,7 @@
         <v>2036</v>
       </c>
       <c r="B48" s="1" t="n">
-        <f aca="false">B47+13</f>
-        <v>594</v>
+        <v>575</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1902,8 +1864,7 @@
         <v>2037</v>
       </c>
       <c r="B49" s="1" t="n">
-        <f aca="false">B48+13</f>
-        <v>607</v>
+        <v>588</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1912,8 +1873,7 @@
         <v>2038</v>
       </c>
       <c r="B50" s="1" t="n">
-        <f aca="false">B49+13</f>
-        <v>620</v>
+        <v>601</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1922,8 +1882,7 @@
         <v>2039</v>
       </c>
       <c r="B51" s="1" t="n">
-        <f aca="false">B50+13</f>
-        <v>633</v>
+        <v>614</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1932,8 +1891,7 @@
         <v>2040</v>
       </c>
       <c r="B52" s="1" t="n">
-        <f aca="false">B51+13</f>
-        <v>646</v>
+        <v>627</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1942,8 +1900,7 @@
         <v>2041</v>
       </c>
       <c r="B53" s="1" t="n">
-        <f aca="false">B52+13</f>
-        <v>659</v>
+        <v>640</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1952,8 +1909,7 @@
         <v>2042</v>
       </c>
       <c r="B54" s="1" t="n">
-        <f aca="false">B53+13</f>
-        <v>672</v>
+        <v>653</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1962,8 +1918,7 @@
         <v>2043</v>
       </c>
       <c r="B55" s="1" t="n">
-        <f aca="false">B54+13</f>
-        <v>685</v>
+        <v>666</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1972,8 +1927,7 @@
         <v>2044</v>
       </c>
       <c r="B56" s="1" t="n">
-        <f aca="false">B55+13</f>
-        <v>698</v>
+        <v>679</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1982,8 +1936,7 @@
         <v>2045</v>
       </c>
       <c r="B57" s="1" t="n">
-        <f aca="false">B56+13</f>
-        <v>711</v>
+        <v>692</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1992,8 +1945,7 @@
         <v>2046</v>
       </c>
       <c r="B58" s="1" t="n">
-        <f aca="false">B57+13</f>
-        <v>724</v>
+        <v>705</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2002,8 +1954,7 @@
         <v>2047</v>
       </c>
       <c r="B59" s="1" t="n">
-        <f aca="false">B58+13</f>
-        <v>737</v>
+        <v>718</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2012,8 +1963,7 @@
         <v>2048</v>
       </c>
       <c r="B60" s="1" t="n">
-        <f aca="false">B59+13</f>
-        <v>750</v>
+        <v>731</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2022,8 +1972,7 @@
         <v>2049</v>
       </c>
       <c r="B61" s="1" t="n">
-        <f aca="false">B60+13</f>
-        <v>763</v>
+        <v>744</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2032,8 +1981,7 @@
         <v>2050</v>
       </c>
       <c r="B62" s="1" t="n">
-        <f aca="false">B61+13</f>
-        <v>776</v>
+        <v>757</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
back to original data
</commit_message>
<xml_diff>
--- a/week_02/data_input/MFA_II_tutorial_II.xlsx
+++ b/week_02/data_input/MFA_II_tutorial_II.xlsx
@@ -504,11 +504,11 @@
           </c:spPr>
         </c:hiLowLines>
         <c:marker val="0"/>
-        <c:axId val="62275712"/>
-        <c:axId val="44196623"/>
+        <c:axId val="12324075"/>
+        <c:axId val="48207983"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="62275712"/>
+        <c:axId val="12324075"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -540,7 +540,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="44196623"/>
+        <c:crossAx val="48207983"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -548,7 +548,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="44196623"/>
+        <c:axId val="48207983"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -587,7 +587,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="62275712"/>
+        <c:crossAx val="12324075"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -626,9 +626,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>12</xdr:col>
-      <xdr:colOff>421200</xdr:colOff>
+      <xdr:colOff>420840</xdr:colOff>
       <xdr:row>19</xdr:row>
-      <xdr:rowOff>3960</xdr:rowOff>
+      <xdr:rowOff>3600</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -637,7 +637,7 @@
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="3769920" y="729720"/>
-        <a:ext cx="4903920" cy="2712600"/>
+        <a:ext cx="4903560" cy="2712240"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -830,7 +830,7 @@
   <dimension ref="A1:D62"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C10" activeCellId="0" sqref="C10"/>
+      <selection pane="topLeft" activeCell="C10" activeCellId="0" sqref="C2:C62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.59765625" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1416,8 +1416,8 @@
   </sheetPr>
   <dimension ref="A1:D62"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A25" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F54" activeCellId="0" sqref="F54"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A40" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2:C62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.59765625" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1441,7 +1441,7 @@
         <v>1990</v>
       </c>
       <c r="B2" s="1" t="n">
-        <v>1</v>
+        <v>20</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1450,7 +1450,7 @@
         <v>1991</v>
       </c>
       <c r="B3" s="1" t="n">
-        <v>2</v>
+        <v>21</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1459,7 +1459,7 @@
         <v>1992</v>
       </c>
       <c r="B4" s="1" t="n">
-        <v>11</v>
+        <v>30</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1468,7 +1468,7 @@
         <v>1993</v>
       </c>
       <c r="B5" s="1" t="n">
-        <v>20</v>
+        <v>39</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1477,7 +1477,7 @@
         <v>1994</v>
       </c>
       <c r="B6" s="1" t="n">
-        <v>26</v>
+        <v>45</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1486,7 +1486,7 @@
         <v>1995</v>
       </c>
       <c r="B7" s="1" t="n">
-        <v>31</v>
+        <v>50</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1495,7 +1495,7 @@
         <v>1996</v>
       </c>
       <c r="B8" s="1" t="n">
-        <v>32</v>
+        <v>51</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1504,7 +1504,7 @@
         <v>1997</v>
       </c>
       <c r="B9" s="1" t="n">
-        <v>33</v>
+        <v>52</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1513,7 +1513,7 @@
         <v>1998</v>
       </c>
       <c r="B10" s="1" t="n">
-        <v>81</v>
+        <v>100</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1522,7 +1522,7 @@
         <v>1999</v>
       </c>
       <c r="B11" s="1" t="n">
-        <v>94</v>
+        <v>113</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1531,7 +1531,7 @@
         <v>2000</v>
       </c>
       <c r="B12" s="1" t="n">
-        <v>107</v>
+        <v>126</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1540,7 +1540,7 @@
         <v>2001</v>
       </c>
       <c r="B13" s="1" t="n">
-        <v>120</v>
+        <v>139</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1549,7 +1549,7 @@
         <v>2002</v>
       </c>
       <c r="B14" s="1" t="n">
-        <v>133</v>
+        <v>152</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1558,7 +1558,7 @@
         <v>2003</v>
       </c>
       <c r="B15" s="1" t="n">
-        <v>146</v>
+        <v>165</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1567,7 +1567,7 @@
         <v>2004</v>
       </c>
       <c r="B16" s="1" t="n">
-        <v>159</v>
+        <v>178</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1576,7 +1576,7 @@
         <v>2005</v>
       </c>
       <c r="B17" s="1" t="n">
-        <v>172</v>
+        <v>191</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1585,7 +1585,7 @@
         <v>2006</v>
       </c>
       <c r="B18" s="1" t="n">
-        <v>185</v>
+        <v>204</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1594,7 +1594,7 @@
         <v>2007</v>
       </c>
       <c r="B19" s="1" t="n">
-        <v>198</v>
+        <v>217</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1603,7 +1603,7 @@
         <v>2008</v>
       </c>
       <c r="B20" s="1" t="n">
-        <v>211</v>
+        <v>230</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1612,7 +1612,7 @@
         <v>2009</v>
       </c>
       <c r="B21" s="1" t="n">
-        <v>224</v>
+        <v>243</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1621,7 +1621,7 @@
         <v>2010</v>
       </c>
       <c r="B22" s="1" t="n">
-        <v>237</v>
+        <v>256</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1630,7 +1630,7 @@
         <v>2011</v>
       </c>
       <c r="B23" s="1" t="n">
-        <v>250</v>
+        <v>269</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1639,7 +1639,7 @@
         <v>2012</v>
       </c>
       <c r="B24" s="1" t="n">
-        <v>263</v>
+        <v>282</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1648,7 +1648,7 @@
         <v>2013</v>
       </c>
       <c r="B25" s="1" t="n">
-        <v>276</v>
+        <v>295</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1657,7 +1657,7 @@
         <v>2014</v>
       </c>
       <c r="B26" s="1" t="n">
-        <v>289</v>
+        <v>308</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1666,7 +1666,7 @@
         <v>2015</v>
       </c>
       <c r="B27" s="1" t="n">
-        <v>302</v>
+        <v>321</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1675,7 +1675,7 @@
         <v>2016</v>
       </c>
       <c r="B28" s="1" t="n">
-        <v>315</v>
+        <v>334</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1684,7 +1684,7 @@
         <v>2017</v>
       </c>
       <c r="B29" s="1" t="n">
-        <v>328</v>
+        <v>347</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1693,7 +1693,7 @@
         <v>2018</v>
       </c>
       <c r="B30" s="1" t="n">
-        <v>341</v>
+        <v>360</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1702,7 +1702,7 @@
         <v>2019</v>
       </c>
       <c r="B31" s="1" t="n">
-        <v>354</v>
+        <v>373</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1711,7 +1711,7 @@
         <v>2020</v>
       </c>
       <c r="B32" s="1" t="n">
-        <v>367</v>
+        <v>386</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1720,7 +1720,7 @@
         <v>2021</v>
       </c>
       <c r="B33" s="1" t="n">
-        <v>380</v>
+        <v>399</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1729,7 +1729,7 @@
         <v>2022</v>
       </c>
       <c r="B34" s="1" t="n">
-        <v>393</v>
+        <v>412</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1738,7 +1738,7 @@
         <v>2023</v>
       </c>
       <c r="B35" s="1" t="n">
-        <v>406</v>
+        <v>425</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1747,7 +1747,7 @@
         <v>2024</v>
       </c>
       <c r="B36" s="1" t="n">
-        <v>419</v>
+        <v>438</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1756,7 +1756,7 @@
         <v>2025</v>
       </c>
       <c r="B37" s="1" t="n">
-        <v>432</v>
+        <v>451</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1765,7 +1765,7 @@
         <v>2026</v>
       </c>
       <c r="B38" s="1" t="n">
-        <v>445</v>
+        <v>464</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1774,7 +1774,7 @@
         <v>2027</v>
       </c>
       <c r="B39" s="1" t="n">
-        <v>458</v>
+        <v>477</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1783,7 +1783,7 @@
         <v>2028</v>
       </c>
       <c r="B40" s="1" t="n">
-        <v>471</v>
+        <v>490</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1792,7 +1792,7 @@
         <v>2029</v>
       </c>
       <c r="B41" s="1" t="n">
-        <v>484</v>
+        <v>503</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1801,7 +1801,7 @@
         <v>2030</v>
       </c>
       <c r="B42" s="1" t="n">
-        <v>497</v>
+        <v>516</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1810,7 +1810,7 @@
         <v>2031</v>
       </c>
       <c r="B43" s="1" t="n">
-        <v>510</v>
+        <v>529</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1819,7 +1819,7 @@
         <v>2032</v>
       </c>
       <c r="B44" s="1" t="n">
-        <v>523</v>
+        <v>542</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1828,7 +1828,7 @@
         <v>2033</v>
       </c>
       <c r="B45" s="1" t="n">
-        <v>536</v>
+        <v>555</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1837,7 +1837,7 @@
         <v>2034</v>
       </c>
       <c r="B46" s="1" t="n">
-        <v>549</v>
+        <v>568</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1846,7 +1846,7 @@
         <v>2035</v>
       </c>
       <c r="B47" s="1" t="n">
-        <v>562</v>
+        <v>581</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1855,7 +1855,7 @@
         <v>2036</v>
       </c>
       <c r="B48" s="1" t="n">
-        <v>575</v>
+        <v>594</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1864,7 +1864,7 @@
         <v>2037</v>
       </c>
       <c r="B49" s="1" t="n">
-        <v>588</v>
+        <v>607</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1873,7 +1873,7 @@
         <v>2038</v>
       </c>
       <c r="B50" s="1" t="n">
-        <v>601</v>
+        <v>620</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1882,7 +1882,7 @@
         <v>2039</v>
       </c>
       <c r="B51" s="1" t="n">
-        <v>614</v>
+        <v>633</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1891,7 +1891,7 @@
         <v>2040</v>
       </c>
       <c r="B52" s="1" t="n">
-        <v>627</v>
+        <v>646</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1900,7 +1900,7 @@
         <v>2041</v>
       </c>
       <c r="B53" s="1" t="n">
-        <v>640</v>
+        <v>659</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1909,7 +1909,7 @@
         <v>2042</v>
       </c>
       <c r="B54" s="1" t="n">
-        <v>653</v>
+        <v>672</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1918,7 +1918,7 @@
         <v>2043</v>
       </c>
       <c r="B55" s="1" t="n">
-        <v>666</v>
+        <v>685</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1927,7 +1927,7 @@
         <v>2044</v>
       </c>
       <c r="B56" s="1" t="n">
-        <v>679</v>
+        <v>698</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1936,7 +1936,7 @@
         <v>2045</v>
       </c>
       <c r="B57" s="1" t="n">
-        <v>692</v>
+        <v>711</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1945,7 +1945,7 @@
         <v>2046</v>
       </c>
       <c r="B58" s="1" t="n">
-        <v>705</v>
+        <v>724</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1954,7 +1954,7 @@
         <v>2047</v>
       </c>
       <c r="B59" s="1" t="n">
-        <v>718</v>
+        <v>737</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1963,7 +1963,7 @@
         <v>2048</v>
       </c>
       <c r="B60" s="1" t="n">
-        <v>731</v>
+        <v>750</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1972,7 +1972,7 @@
         <v>2049</v>
       </c>
       <c r="B61" s="1" t="n">
-        <v>744</v>
+        <v>763</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1981,7 +1981,7 @@
         <v>2050</v>
       </c>
       <c r="B62" s="1" t="n">
-        <v>757</v>
+        <v>776</v>
       </c>
     </row>
   </sheetData>

</xml_diff>